<commit_message>
Update ATACseq assay re meeting with Stanford
</commit_message>
<xml_diff>
--- a/template_examples/atacseq_fastq_template.xlsx
+++ b/template_examples/atacseq_fastq_template.xlsx
@@ -221,7 +221,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">quantitative measure of the sequencing libraries quality</t>
+          <t xml:space="preserve">One quantitative measure of the sequencing accuracy.</t>
         </r>
       </text>
     </comment>
@@ -318,7 +318,7 @@
     <t xml:space="preserve">Sequencing date</t>
   </si>
   <si>
-    <t xml:space="preserve">Dv200</t>
+    <t xml:space="preserve">%q30</t>
   </si>
   <si>
     <t xml:space="preserve">Quality flag</t>
@@ -429,7 +429,7 @@
     <t xml:space="preserve">Number</t>
   </si>
   <si>
-    <t xml:space="preserve">quantitative measure of the sequencing libraries quality</t>
+    <t xml:space="preserve">One quantitative measure of the sequencing accuracy.</t>
   </si>
   <si>
     <t xml:space="preserve">Flag used for quality.</t>
@@ -701,8 +701,8 @@
   </sheetPr>
   <dimension ref="A1:I2012"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -868,7 +868,7 @@
         <v>40179</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="I13" s="4" t="n">
         <v>1</v>
@@ -897,7 +897,7 @@
         <v>40179</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="I14" s="4" t="n">
         <v>1</v>
@@ -926,7 +926,7 @@
         <v>40179</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="I15" s="4" t="n">
         <v>1</v>
@@ -955,7 +955,7 @@
         <v>40179</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="I16" s="4" t="n">
         <v>1</v>

</xml_diff>